<commit_message>
Añadiendo las horas de trabajo para HU-1 Y HU-2
</commit_message>
<xml_diff>
--- a/Scrum-Project-Management.xlsx
+++ b/Scrum-Project-Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Cursos 9no semestre\Taller de proyectos 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Cursos 9no semestre\Taller de proyectos 1\IDEA-PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA18670F-470A-4B1D-85FF-3C5E6BA5C732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3811CC63-30A2-4612-962D-9E0DD8643056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LO Diagrama de Gantt y Burndown" sheetId="1" r:id="rId1"/>
@@ -2472,6 +2472,34 @@
     <xf numFmtId="0" fontId="37" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2492,7 +2520,6 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2500,8 +2527,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2520,31 +2545,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5383,9 +5383,9 @@
   </sheetPr>
   <dimension ref="A1:BV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -5509,7 +5509,7 @@
       <c r="H3" s="40"/>
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
-      <c r="K3" s="236" t="s">
+      <c r="K3" s="250" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="42" t="s">
@@ -5588,7 +5588,7 @@
       <c r="H4" s="40"/>
       <c r="I4" s="40"/>
       <c r="J4" s="41"/>
-      <c r="K4" s="237"/>
+      <c r="K4" s="251"/>
       <c r="L4" s="47" t="s">
         <v>3</v>
       </c>
@@ -5665,7 +5665,7 @@
       <c r="H5" s="37"/>
       <c r="I5" s="36"/>
       <c r="J5" s="37"/>
-      <c r="K5" s="237"/>
+      <c r="K5" s="251"/>
       <c r="L5" s="52" t="s">
         <v>4</v>
       </c>
@@ -5742,7 +5742,7 @@
       <c r="H6" s="37"/>
       <c r="I6" s="36"/>
       <c r="J6" s="37"/>
-      <c r="K6" s="237"/>
+      <c r="K6" s="251"/>
       <c r="L6" s="54" t="s">
         <v>5</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="H7" s="37"/>
       <c r="I7" s="36"/>
       <c r="J7" s="37"/>
-      <c r="K7" s="238"/>
+      <c r="K7" s="252"/>
       <c r="L7" s="56" t="s">
         <v>6</v>
       </c>
@@ -5887,122 +5887,122 @@
       <c r="BV7" s="39"/>
     </row>
     <row r="8" spans="1:74" ht="23.1" customHeight="1">
-      <c r="B8" s="253" t="s">
+      <c r="B8" s="233" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="261" t="s">
+      <c r="C8" s="242" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="257" t="s">
+      <c r="D8" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="233" t="s">
+      <c r="E8" s="247" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="234"/>
-      <c r="G8" s="235"/>
-      <c r="H8" s="255" t="s">
+      <c r="F8" s="248"/>
+      <c r="G8" s="249"/>
+      <c r="H8" s="235" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="259" t="s">
+      <c r="I8" s="239" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="260" t="s">
+      <c r="J8" s="240" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="239" t="s">
+      <c r="K8" s="253" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="241" t="s">
+      <c r="L8" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="243" t="s">
+      <c r="M8" s="256" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="244"/>
-      <c r="O8" s="244"/>
-      <c r="P8" s="244"/>
-      <c r="Q8" s="245"/>
-      <c r="R8" s="246" t="s">
+      <c r="N8" s="231"/>
+      <c r="O8" s="231"/>
+      <c r="P8" s="231"/>
+      <c r="Q8" s="232"/>
+      <c r="R8" s="257" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="244"/>
-      <c r="T8" s="244"/>
-      <c r="U8" s="244"/>
-      <c r="V8" s="245"/>
-      <c r="W8" s="246" t="s">
+      <c r="S8" s="231"/>
+      <c r="T8" s="231"/>
+      <c r="U8" s="231"/>
+      <c r="V8" s="232"/>
+      <c r="W8" s="257" t="s">
         <v>18</v>
       </c>
-      <c r="X8" s="244"/>
-      <c r="Y8" s="244"/>
-      <c r="Z8" s="244"/>
-      <c r="AA8" s="245"/>
-      <c r="AB8" s="248" t="s">
+      <c r="X8" s="231"/>
+      <c r="Y8" s="231"/>
+      <c r="Z8" s="231"/>
+      <c r="AA8" s="232"/>
+      <c r="AB8" s="259" t="s">
         <v>19</v>
       </c>
-      <c r="AC8" s="244"/>
-      <c r="AD8" s="244"/>
-      <c r="AE8" s="244"/>
-      <c r="AF8" s="245"/>
-      <c r="AG8" s="249" t="s">
+      <c r="AC8" s="231"/>
+      <c r="AD8" s="231"/>
+      <c r="AE8" s="231"/>
+      <c r="AF8" s="232"/>
+      <c r="AG8" s="260" t="s">
         <v>20</v>
       </c>
-      <c r="AH8" s="244"/>
-      <c r="AI8" s="244"/>
-      <c r="AJ8" s="244"/>
-      <c r="AK8" s="245"/>
-      <c r="AL8" s="249" t="s">
+      <c r="AH8" s="231"/>
+      <c r="AI8" s="231"/>
+      <c r="AJ8" s="231"/>
+      <c r="AK8" s="232"/>
+      <c r="AL8" s="260" t="s">
         <v>21</v>
       </c>
-      <c r="AM8" s="244"/>
-      <c r="AN8" s="244"/>
-      <c r="AO8" s="244"/>
-      <c r="AP8" s="245"/>
-      <c r="AQ8" s="247" t="s">
+      <c r="AM8" s="231"/>
+      <c r="AN8" s="231"/>
+      <c r="AO8" s="231"/>
+      <c r="AP8" s="232"/>
+      <c r="AQ8" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="AR8" s="244"/>
-      <c r="AS8" s="244"/>
-      <c r="AT8" s="244"/>
-      <c r="AU8" s="245"/>
-      <c r="AV8" s="250" t="s">
+      <c r="AR8" s="231"/>
+      <c r="AS8" s="231"/>
+      <c r="AT8" s="231"/>
+      <c r="AU8" s="232"/>
+      <c r="AV8" s="261" t="s">
         <v>23</v>
       </c>
-      <c r="AW8" s="244"/>
-      <c r="AX8" s="244"/>
-      <c r="AY8" s="244"/>
-      <c r="AZ8" s="245"/>
-      <c r="BA8" s="250" t="s">
+      <c r="AW8" s="231"/>
+      <c r="AX8" s="231"/>
+      <c r="AY8" s="231"/>
+      <c r="AZ8" s="232"/>
+      <c r="BA8" s="261" t="s">
         <v>24</v>
       </c>
-      <c r="BB8" s="244"/>
-      <c r="BC8" s="244"/>
-      <c r="BD8" s="244"/>
-      <c r="BE8" s="245"/>
-      <c r="BF8" s="251" t="s">
+      <c r="BB8" s="231"/>
+      <c r="BC8" s="231"/>
+      <c r="BD8" s="231"/>
+      <c r="BE8" s="232"/>
+      <c r="BF8" s="262" t="s">
         <v>25</v>
       </c>
-      <c r="BG8" s="244"/>
-      <c r="BH8" s="244"/>
-      <c r="BI8" s="244"/>
-      <c r="BJ8" s="245"/>
-      <c r="BK8" s="252"/>
-      <c r="BL8" s="244"/>
-      <c r="BM8" s="244"/>
-      <c r="BN8" s="244"/>
-      <c r="BO8" s="245"/>
-      <c r="BP8" s="252"/>
-      <c r="BQ8" s="244"/>
-      <c r="BR8" s="244"/>
-      <c r="BS8" s="244"/>
-      <c r="BT8" s="245"/>
+      <c r="BG8" s="231"/>
+      <c r="BH8" s="231"/>
+      <c r="BI8" s="231"/>
+      <c r="BJ8" s="232"/>
+      <c r="BK8" s="230"/>
+      <c r="BL8" s="231"/>
+      <c r="BM8" s="231"/>
+      <c r="BN8" s="231"/>
+      <c r="BO8" s="232"/>
+      <c r="BP8" s="230"/>
+      <c r="BQ8" s="231"/>
+      <c r="BR8" s="231"/>
+      <c r="BS8" s="231"/>
+      <c r="BT8" s="232"/>
       <c r="BU8" s="38"/>
       <c r="BV8" s="39"/>
     </row>
     <row r="9" spans="1:74" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B9" s="254"/>
-      <c r="C9" s="262"/>
-      <c r="D9" s="258"/>
+      <c r="B9" s="234"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="238"/>
       <c r="E9" s="58" t="s">
         <v>28</v>
       </c>
@@ -6012,11 +6012,11 @@
       <c r="G9" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="256"/>
-      <c r="I9" s="245"/>
-      <c r="J9" s="240"/>
-      <c r="K9" s="240"/>
-      <c r="L9" s="242"/>
+      <c r="H9" s="236"/>
+      <c r="I9" s="232"/>
+      <c r="J9" s="241"/>
+      <c r="K9" s="241"/>
+      <c r="L9" s="255"/>
       <c r="M9" s="61" t="s">
         <v>31</v>
       </c>
@@ -8487,12 +8487,10 @@
         <v>4</v>
       </c>
       <c r="F35" s="198">
-        <f>SUM(F36:F39)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G35" s="199">
-        <f>SUM(G36:G39)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H35" s="200"/>
       <c r="I35" s="206">
@@ -8507,7 +8505,7 @@
       </c>
       <c r="L35" s="201">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="M35" s="73"/>
       <c r="N35" s="74"/>
@@ -8677,11 +8675,11 @@
         <v>1</v>
       </c>
       <c r="F37" s="154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="155">
         <f>E37-F37</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="212"/>
       <c r="I37" s="157"/>
@@ -8689,7 +8687,7 @@
       <c r="K37" s="213"/>
       <c r="L37" s="201">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="73"/>
       <c r="N37" s="74"/>
@@ -8768,11 +8766,11 @@
         <v>1</v>
       </c>
       <c r="F38" s="154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="155">
         <f>E38-F38</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="212"/>
       <c r="I38" s="157"/>
@@ -8780,7 +8778,7 @@
       <c r="K38" s="213"/>
       <c r="L38" s="201">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="73"/>
       <c r="N38" s="74"/>
@@ -8859,11 +8857,11 @@
         <v>1</v>
       </c>
       <c r="F39" s="220">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="190">
         <f>E39-F39</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="221"/>
       <c r="I39" s="222"/>
@@ -8871,7 +8869,7 @@
       <c r="K39" s="214"/>
       <c r="L39" s="201">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="73"/>
       <c r="N39" s="74"/>
@@ -9035,11 +9033,11 @@
       </c>
       <c r="F41" s="216">
         <f>SUM(F11:F14,F16:F19,F21:F24,F26:F29,F31:F34,F36:F39)</f>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G41" s="216">
         <f>SUM(G11:G14,G16:G19,G21:G24,G26:G29,G31:G34,G36:G39)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H41" s="217">
         <v>7</v>
@@ -9541,89 +9539,82 @@
     <row r="47" spans="2:74" ht="381.95" customHeight="1"/>
     <row r="48" spans="2:74" ht="216.95" customHeight="1"/>
     <row r="50" spans="2:74" ht="50.1" customHeight="1">
-      <c r="B50" s="230"/>
-      <c r="C50" s="231"/>
-      <c r="D50" s="231"/>
-      <c r="E50" s="231"/>
-      <c r="F50" s="231"/>
-      <c r="G50" s="231"/>
-      <c r="H50" s="231"/>
-      <c r="I50" s="231"/>
-      <c r="J50" s="231"/>
-      <c r="K50" s="231"/>
-      <c r="L50" s="231"/>
-      <c r="M50" s="231"/>
-      <c r="N50" s="231"/>
-      <c r="O50" s="231"/>
-      <c r="P50" s="231"/>
-      <c r="Q50" s="231"/>
-      <c r="R50" s="231"/>
-      <c r="S50" s="231"/>
-      <c r="T50" s="231"/>
-      <c r="U50" s="231"/>
-      <c r="V50" s="231"/>
-      <c r="W50" s="231"/>
-      <c r="X50" s="231"/>
-      <c r="Y50" s="231"/>
-      <c r="Z50" s="231"/>
-      <c r="AA50" s="231"/>
-      <c r="AB50" s="231"/>
-      <c r="AC50" s="231"/>
-      <c r="AD50" s="231"/>
-      <c r="AE50" s="231"/>
-      <c r="AF50" s="231"/>
-      <c r="AG50" s="231"/>
-      <c r="AH50" s="231"/>
-      <c r="AI50" s="231"/>
-      <c r="AJ50" s="231"/>
-      <c r="AK50" s="231"/>
-      <c r="AL50" s="231"/>
-      <c r="AM50" s="231"/>
-      <c r="AN50" s="231"/>
-      <c r="AO50" s="231"/>
-      <c r="AP50" s="231"/>
-      <c r="AQ50" s="231"/>
-      <c r="AR50" s="231"/>
-      <c r="AS50" s="231"/>
-      <c r="AT50" s="231"/>
-      <c r="AU50" s="231"/>
-      <c r="AV50" s="231"/>
-      <c r="AW50" s="231"/>
-      <c r="AX50" s="231"/>
-      <c r="AY50" s="231"/>
-      <c r="AZ50" s="231"/>
-      <c r="BA50" s="231"/>
-      <c r="BB50" s="231"/>
-      <c r="BC50" s="231"/>
-      <c r="BD50" s="231"/>
-      <c r="BE50" s="231"/>
-      <c r="BF50" s="231"/>
-      <c r="BG50" s="231"/>
-      <c r="BH50" s="231"/>
-      <c r="BI50" s="231"/>
-      <c r="BJ50" s="231"/>
-      <c r="BK50" s="231"/>
-      <c r="BL50" s="231"/>
-      <c r="BM50" s="231"/>
-      <c r="BN50" s="231"/>
-      <c r="BO50" s="231"/>
-      <c r="BP50" s="231"/>
-      <c r="BQ50" s="231"/>
-      <c r="BR50" s="231"/>
-      <c r="BS50" s="231"/>
-      <c r="BT50" s="231"/>
-      <c r="BU50" s="231"/>
-      <c r="BV50" s="232"/>
+      <c r="B50" s="244"/>
+      <c r="C50" s="245"/>
+      <c r="D50" s="245"/>
+      <c r="E50" s="245"/>
+      <c r="F50" s="245"/>
+      <c r="G50" s="245"/>
+      <c r="H50" s="245"/>
+      <c r="I50" s="245"/>
+      <c r="J50" s="245"/>
+      <c r="K50" s="245"/>
+      <c r="L50" s="245"/>
+      <c r="M50" s="245"/>
+      <c r="N50" s="245"/>
+      <c r="O50" s="245"/>
+      <c r="P50" s="245"/>
+      <c r="Q50" s="245"/>
+      <c r="R50" s="245"/>
+      <c r="S50" s="245"/>
+      <c r="T50" s="245"/>
+      <c r="U50" s="245"/>
+      <c r="V50" s="245"/>
+      <c r="W50" s="245"/>
+      <c r="X50" s="245"/>
+      <c r="Y50" s="245"/>
+      <c r="Z50" s="245"/>
+      <c r="AA50" s="245"/>
+      <c r="AB50" s="245"/>
+      <c r="AC50" s="245"/>
+      <c r="AD50" s="245"/>
+      <c r="AE50" s="245"/>
+      <c r="AF50" s="245"/>
+      <c r="AG50" s="245"/>
+      <c r="AH50" s="245"/>
+      <c r="AI50" s="245"/>
+      <c r="AJ50" s="245"/>
+      <c r="AK50" s="245"/>
+      <c r="AL50" s="245"/>
+      <c r="AM50" s="245"/>
+      <c r="AN50" s="245"/>
+      <c r="AO50" s="245"/>
+      <c r="AP50" s="245"/>
+      <c r="AQ50" s="245"/>
+      <c r="AR50" s="245"/>
+      <c r="AS50" s="245"/>
+      <c r="AT50" s="245"/>
+      <c r="AU50" s="245"/>
+      <c r="AV50" s="245"/>
+      <c r="AW50" s="245"/>
+      <c r="AX50" s="245"/>
+      <c r="AY50" s="245"/>
+      <c r="AZ50" s="245"/>
+      <c r="BA50" s="245"/>
+      <c r="BB50" s="245"/>
+      <c r="BC50" s="245"/>
+      <c r="BD50" s="245"/>
+      <c r="BE50" s="245"/>
+      <c r="BF50" s="245"/>
+      <c r="BG50" s="245"/>
+      <c r="BH50" s="245"/>
+      <c r="BI50" s="245"/>
+      <c r="BJ50" s="245"/>
+      <c r="BK50" s="245"/>
+      <c r="BL50" s="245"/>
+      <c r="BM50" s="245"/>
+      <c r="BN50" s="245"/>
+      <c r="BO50" s="245"/>
+      <c r="BP50" s="245"/>
+      <c r="BQ50" s="245"/>
+      <c r="BR50" s="245"/>
+      <c r="BS50" s="245"/>
+      <c r="BT50" s="245"/>
+      <c r="BU50" s="245"/>
+      <c r="BV50" s="246"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="BP8:BT8"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="B50:BV50"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="K3:K7"/>
@@ -9640,6 +9631,13 @@
     <mergeCell ref="BA8:BE8"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
+    <mergeCell ref="BP8:BT8"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <conditionalFormatting sqref="L10">
@@ -9754,8 +9752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097109D2-447F-4F39-A4BD-92E74C4EFF49}">
   <dimension ref="B3:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -9846,10 +9844,10 @@
         <v>127</v>
       </c>
       <c r="C9" s="209"/>
-      <c r="D9" s="228" t="s">
+      <c r="D9" s="209"/>
+      <c r="E9" s="228" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="209"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9972,7 +9970,7 @@
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
       <c r="J2" s="41"/>
-      <c r="K2" s="236" t="s">
+      <c r="K2" s="250" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="42" t="s">
@@ -10051,7 +10049,7 @@
       <c r="H3" s="40"/>
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
-      <c r="K3" s="237"/>
+      <c r="K3" s="251"/>
       <c r="L3" s="47" t="s">
         <v>3</v>
       </c>
@@ -10128,7 +10126,7 @@
       <c r="H4" s="37"/>
       <c r="I4" s="36"/>
       <c r="J4" s="37"/>
-      <c r="K4" s="237"/>
+      <c r="K4" s="251"/>
       <c r="L4" s="52" t="s">
         <v>4</v>
       </c>
@@ -10205,7 +10203,7 @@
       <c r="H5" s="37"/>
       <c r="I5" s="36"/>
       <c r="J5" s="37"/>
-      <c r="K5" s="237"/>
+      <c r="K5" s="251"/>
       <c r="L5" s="54" t="s">
         <v>5</v>
       </c>
@@ -10282,7 +10280,7 @@
       <c r="H6" s="37"/>
       <c r="I6" s="36"/>
       <c r="J6" s="37"/>
-      <c r="K6" s="238"/>
+      <c r="K6" s="252"/>
       <c r="L6" s="56" t="s">
         <v>6</v>
       </c>
@@ -10350,126 +10348,126 @@
       <c r="BV6" s="39"/>
     </row>
     <row r="7" spans="2:74" ht="23.1" customHeight="1">
-      <c r="B7" s="253" t="s">
+      <c r="B7" s="233" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="261" t="s">
+      <c r="C7" s="242" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="257" t="s">
+      <c r="D7" s="237" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="247" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="234"/>
-      <c r="G7" s="235"/>
-      <c r="H7" s="255" t="s">
+      <c r="F7" s="248"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="235" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="259" t="s">
+      <c r="I7" s="239" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="260" t="s">
+      <c r="J7" s="240" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="239" t="s">
+      <c r="K7" s="253" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="241" t="s">
+      <c r="L7" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="243" t="s">
+      <c r="M7" s="256" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="244"/>
-      <c r="O7" s="244"/>
-      <c r="P7" s="244"/>
-      <c r="Q7" s="245"/>
-      <c r="R7" s="246" t="s">
+      <c r="N7" s="231"/>
+      <c r="O7" s="231"/>
+      <c r="P7" s="231"/>
+      <c r="Q7" s="232"/>
+      <c r="R7" s="257" t="s">
         <v>17</v>
       </c>
-      <c r="S7" s="244"/>
-      <c r="T7" s="244"/>
-      <c r="U7" s="244"/>
-      <c r="V7" s="245"/>
-      <c r="W7" s="246" t="s">
+      <c r="S7" s="231"/>
+      <c r="T7" s="231"/>
+      <c r="U7" s="231"/>
+      <c r="V7" s="232"/>
+      <c r="W7" s="257" t="s">
         <v>18</v>
       </c>
-      <c r="X7" s="244"/>
-      <c r="Y7" s="244"/>
-      <c r="Z7" s="244"/>
-      <c r="AA7" s="245"/>
-      <c r="AB7" s="248" t="s">
+      <c r="X7" s="231"/>
+      <c r="Y7" s="231"/>
+      <c r="Z7" s="231"/>
+      <c r="AA7" s="232"/>
+      <c r="AB7" s="259" t="s">
         <v>19</v>
       </c>
-      <c r="AC7" s="244"/>
-      <c r="AD7" s="244"/>
-      <c r="AE7" s="244"/>
-      <c r="AF7" s="245"/>
-      <c r="AG7" s="249" t="s">
+      <c r="AC7" s="231"/>
+      <c r="AD7" s="231"/>
+      <c r="AE7" s="231"/>
+      <c r="AF7" s="232"/>
+      <c r="AG7" s="260" t="s">
         <v>20</v>
       </c>
-      <c r="AH7" s="244"/>
-      <c r="AI7" s="244"/>
-      <c r="AJ7" s="244"/>
-      <c r="AK7" s="245"/>
-      <c r="AL7" s="249" t="s">
+      <c r="AH7" s="231"/>
+      <c r="AI7" s="231"/>
+      <c r="AJ7" s="231"/>
+      <c r="AK7" s="232"/>
+      <c r="AL7" s="260" t="s">
         <v>21</v>
       </c>
-      <c r="AM7" s="244"/>
-      <c r="AN7" s="244"/>
-      <c r="AO7" s="244"/>
-      <c r="AP7" s="245"/>
-      <c r="AQ7" s="247" t="s">
+      <c r="AM7" s="231"/>
+      <c r="AN7" s="231"/>
+      <c r="AO7" s="231"/>
+      <c r="AP7" s="232"/>
+      <c r="AQ7" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="AR7" s="244"/>
-      <c r="AS7" s="244"/>
-      <c r="AT7" s="244"/>
-      <c r="AU7" s="245"/>
-      <c r="AV7" s="250" t="s">
+      <c r="AR7" s="231"/>
+      <c r="AS7" s="231"/>
+      <c r="AT7" s="231"/>
+      <c r="AU7" s="232"/>
+      <c r="AV7" s="261" t="s">
         <v>23</v>
       </c>
-      <c r="AW7" s="244"/>
-      <c r="AX7" s="244"/>
-      <c r="AY7" s="244"/>
-      <c r="AZ7" s="245"/>
-      <c r="BA7" s="250" t="s">
+      <c r="AW7" s="231"/>
+      <c r="AX7" s="231"/>
+      <c r="AY7" s="231"/>
+      <c r="AZ7" s="232"/>
+      <c r="BA7" s="261" t="s">
         <v>24</v>
       </c>
-      <c r="BB7" s="244"/>
-      <c r="BC7" s="244"/>
-      <c r="BD7" s="244"/>
-      <c r="BE7" s="245"/>
-      <c r="BF7" s="251" t="s">
+      <c r="BB7" s="231"/>
+      <c r="BC7" s="231"/>
+      <c r="BD7" s="231"/>
+      <c r="BE7" s="232"/>
+      <c r="BF7" s="262" t="s">
         <v>25</v>
       </c>
-      <c r="BG7" s="244"/>
-      <c r="BH7" s="244"/>
-      <c r="BI7" s="244"/>
-      <c r="BJ7" s="245"/>
+      <c r="BG7" s="231"/>
+      <c r="BH7" s="231"/>
+      <c r="BI7" s="231"/>
+      <c r="BJ7" s="232"/>
       <c r="BK7" s="263" t="s">
         <v>26</v>
       </c>
-      <c r="BL7" s="244"/>
-      <c r="BM7" s="244"/>
-      <c r="BN7" s="244"/>
-      <c r="BO7" s="245"/>
+      <c r="BL7" s="231"/>
+      <c r="BM7" s="231"/>
+      <c r="BN7" s="231"/>
+      <c r="BO7" s="232"/>
       <c r="BP7" s="263" t="s">
         <v>27</v>
       </c>
-      <c r="BQ7" s="244"/>
-      <c r="BR7" s="244"/>
-      <c r="BS7" s="244"/>
-      <c r="BT7" s="245"/>
+      <c r="BQ7" s="231"/>
+      <c r="BR7" s="231"/>
+      <c r="BS7" s="231"/>
+      <c r="BT7" s="232"/>
       <c r="BU7" s="38"/>
       <c r="BV7" s="39"/>
     </row>
     <row r="8" spans="2:74" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B8" s="254"/>
-      <c r="C8" s="262"/>
-      <c r="D8" s="258"/>
+      <c r="B8" s="234"/>
+      <c r="C8" s="243"/>
+      <c r="D8" s="238"/>
       <c r="E8" s="58" t="s">
         <v>28</v>
       </c>
@@ -10479,11 +10477,11 @@
       <c r="G8" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="256"/>
-      <c r="I8" s="245"/>
-      <c r="J8" s="240"/>
-      <c r="K8" s="240"/>
-      <c r="L8" s="242"/>
+      <c r="H8" s="236"/>
+      <c r="I8" s="232"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="241"/>
+      <c r="L8" s="255"/>
       <c r="M8" s="61" t="s">
         <v>31</v>
       </c>
@@ -14003,6 +14001,13 @@
     <row r="42" spans="2:74" ht="216.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="BP7:BT7"/>
+    <mergeCell ref="AL7:AP7"/>
+    <mergeCell ref="AQ7:AU7"/>
+    <mergeCell ref="AV7:AZ7"/>
+    <mergeCell ref="BA7:BE7"/>
+    <mergeCell ref="BF7:BJ7"/>
+    <mergeCell ref="BK7:BO7"/>
     <mergeCell ref="AG7:AK7"/>
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="B7:B8"/>
@@ -14018,13 +14023,6 @@
     <mergeCell ref="R7:V7"/>
     <mergeCell ref="W7:AA7"/>
     <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="BP7:BT7"/>
-    <mergeCell ref="AL7:AP7"/>
-    <mergeCell ref="AQ7:AU7"/>
-    <mergeCell ref="AV7:AZ7"/>
-    <mergeCell ref="BA7:BE7"/>
-    <mergeCell ref="BF7:BJ7"/>
-    <mergeCell ref="BK7:BO7"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:L33">
     <cfRule type="dataBar" priority="1">

</xml_diff>